<commit_message>
saving RES generation in yearly excels
</commit_message>
<xml_diff>
--- a/data/exported_Traderes.xlsx
+++ b/data/exported_Traderes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B31E26-CC19-4370-9DF8-B17F32226862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F686702-371B-4667-95F8-25BDB80BE5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" tabRatio="977" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={5440F79C-069D-4630-B655-D51101D93DC9}</author>
-    <author>tc={9554A1FD-F317-4BB3-A1FC-ACD61C221824}</author>
   </authors>
   <commentList>
     <comment ref="C12" authorId="0" shapeId="0" xr:uid="{5440F79C-069D-4630-B655-D51101D93DC9}">
@@ -62,14 +61,6 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     changed from base to 2040</t>
-      </text>
-    </comment>
-    <comment ref="D61" authorId="1" shapeId="0" xr:uid="{9554A1FD-F317-4BB3-A1FC-ACD61C221824}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    20.16</t>
       </text>
     </comment>
   </commentList>
@@ -800,7 +791,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,12 +877,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -6615,9 +6600,6 @@
   <threadedComment ref="C12" dT="2022-03-14T19:51:52.93" personId="{08DB7B5E-EE37-4573-9C2A-FF3EA7A96B25}" id="{5440F79C-069D-4630-B655-D51101D93DC9}">
     <text>changed from base to 2040</text>
   </threadedComment>
-  <threadedComment ref="D61" dT="2022-10-24T19:30:10.30" personId="{08DB7B5E-EE37-4573-9C2A-FF3EA7A96B25}" id="{9554A1FD-F317-4BB3-A1FC-ACD61C221824}">
-    <text>20.16</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -28815,8 +28797,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -29711,7 +29693,7 @@
         <v>83</v>
       </c>
       <c r="D61" s="8">
-        <v>120</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="62" spans="1:4">

</xml_diff>

<commit_message>
adding amiris data structure template
</commit_message>
<xml_diff>
--- a/data/exported_Traderes.xlsx
+++ b/data/exported_Traderes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F686702-371B-4667-95F8-25BDB80BE5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6220EB50-4A95-4FCE-9694-59C9D5F9D870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" tabRatio="977" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="977" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grid" sheetId="1" r:id="rId1"/>
@@ -135,6 +135,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={0815C989-6CA7-4603-8C5B-192E23334E1A}</author>
+    <author>tc={D2699E04-0851-4D4C-8020-4EADA78C466D}</author>
   </authors>
   <commentList>
     <comment ref="I46" authorId="0" shapeId="0" xr:uid="{0815C989-6CA7-4603-8C5B-192E23334E1A}">
@@ -143,6 +144,15 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Was 40
+</t>
+      </text>
+    </comment>
+    <comment ref="K52" authorId="1" shapeId="0" xr:uid="{D2699E04-0851-4D4C-8020-4EADA78C466D}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is from MIT
 </t>
       </text>
     </comment>
@@ -791,7 +801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,6 +887,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -6635,6 +6651,10 @@
     <text xml:space="preserve">Was 40
 </text>
   </threadedComment>
+  <threadedComment ref="K52" dT="2022-10-25T14:44:30.68" personId="{08DB7B5E-EE37-4573-9C2A-FF3EA7A96B25}" id="{D2699E04-0851-4D4C-8020-4EADA78C466D}">
+    <text xml:space="preserve">This is from MIT
+</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -28797,8 +28817,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -30038,8 +30058,8 @@
   </sheetPr>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -30335,8 +30355,9 @@
     <hyperlink ref="O2" r:id="rId4" xr:uid="{97BF3871-2C9F-4A98-8C67-66B6773BB269}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -30347,8 +30368,8 @@
   </sheetPr>
   <dimension ref="A1:DI57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="V60" sqref="V60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -32878,6 +32899,18 @@
       <c r="I52" s="18">
         <v>20</v>
       </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>0.92</v>
+      </c>
+      <c r="L52">
+        <v>0.92</v>
+      </c>
+      <c r="M52" s="18">
+        <v>0</v>
+      </c>
       <c r="Y52"/>
       <c r="Z52"/>
       <c r="AA52"/>

</xml_diff>

<commit_message>
not allowing fossil fueled in CRM
</commit_message>
<xml_diff>
--- a/data/exported_Traderes.xlsx
+++ b/data/exported_Traderes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD9ED71-18B5-48DA-BD0A-0F5BC25DC391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6CA2D8-4F11-4E4D-894A-AA9E1138C86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="917" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="917" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="explanation" sheetId="1" r:id="rId1"/>
@@ -1994,7 +1994,7 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="90" wrapText="1"/>
@@ -2150,9 +2150,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Comma" xfId="11" builtinId="3"/>
@@ -32869,8 +32867,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32911,7 +32909,7 @@
       <c r="B3">
         <v>2050</v>
       </c>
-      <c r="C3" s="50">
+      <c r="C3" s="109">
         <v>350000</v>
       </c>
     </row>
@@ -32971,27 +32969,27 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="116" t="s">
+      <c r="A9" s="115" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="116">
+      <c r="B9" s="115">
         <v>2050</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="109">
         <v>360000</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="115" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="116">
+      <c r="B10" s="115">
         <v>2050</v>
       </c>
-      <c r="C10" s="117">
+      <c r="C10" s="109">
         <v>7940450</v>
       </c>
-      <c r="D10" s="116"/>
+      <c r="D10" s="115"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="114" t="s">
@@ -33044,7 +33042,7 @@
       <c r="B15" s="5">
         <v>2050</v>
       </c>
-      <c r="C15" s="115">
+      <c r="C15" s="109">
         <v>1040000</v>
       </c>
     </row>
@@ -33055,7 +33053,7 @@
       <c r="B16" s="5">
         <v>2050</v>
       </c>
-      <c r="C16" s="115">
+      <c r="C16" s="109">
         <v>412000</v>
       </c>
     </row>
@@ -33074,10 +33072,10 @@
   <sheetPr>
     <tabColor rgb="FFE945D2"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33085,7 +33083,7 @@
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -33093,130 +33091,125 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="116" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="116">
+      <c r="B2">
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="116" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>299</v>
       </c>
-      <c r="B3" s="116">
+      <c r="B3">
         <v>9500</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="116" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>300</v>
       </c>
       <c r="B4">
         <v>10700</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="116" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>301</v>
       </c>
-      <c r="B5" s="116">
+      <c r="B5">
         <v>12600</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="116" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>305</v>
       </c>
-      <c r="B6" s="116">
+      <c r="B6">
         <v>39000</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="116" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="116">
+      <c r="B7">
         <v>111166.3</v>
       </c>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="116" t="s">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>304</v>
       </c>
-      <c r="B8" s="116">
+      <c r="B8">
         <v>64000</v>
       </c>
-      <c r="C8" s="116"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="110" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>308</v>
       </c>
       <c r="B9">
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="110" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>309</v>
       </c>
       <c r="B10">
         <v>20000</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11">
         <v>14950</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>310</v>
       </c>
-      <c r="B12" s="105">
+      <c r="B12">
         <v>30000</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>311</v>
       </c>
-      <c r="B13" s="105">
+      <c r="B13">
         <v>11250</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>312</v>
       </c>
-      <c r="B14" s="105">
+      <c r="B14">
         <v>8700</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="105">
+      <c r="B15">
         <v>7000</v>
       </c>
-      <c r="C15" s="105"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="105">
+      <c r="B16">
         <v>7423</v>
       </c>
-      <c r="C16" s="105"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
@@ -33239,7 +33232,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33474,8 +33467,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33487,13 +33480,13 @@
       <c r="A1" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" t="s">
         <v>213</v>
       </c>
       <c r="E1" s="60" t="s">
@@ -33622,55 +33615,55 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="116" t="s">
+      <c r="A7" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="116">
+      <c r="B7">
         <v>3.5</v>
       </c>
-      <c r="C7" s="116">
+      <c r="C7">
         <v>0.35</v>
       </c>
-      <c r="D7" s="116">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="116">
+      <c r="E7" s="115">
         <v>0</v>
       </c>
-      <c r="F7" s="116">
+      <c r="F7" s="115">
         <v>0</v>
       </c>
-      <c r="G7" s="116">
+      <c r="G7" s="115">
         <v>0</v>
       </c>
-      <c r="H7" s="116"/>
+      <c r="H7" s="115"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="116" t="s">
+      <c r="A8" t="s">
         <v>304</v>
       </c>
-      <c r="B8" s="116">
+      <c r="B8">
         <v>2.6</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8">
         <v>0.309</v>
       </c>
-      <c r="D8" s="116">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="116">
+      <c r="E8" s="115">
         <v>0</v>
       </c>
-      <c r="F8" s="116">
+      <c r="F8" s="115">
         <v>0</v>
       </c>
-      <c r="G8" s="116">
+      <c r="G8" s="115">
         <v>0</v>
       </c>
-      <c r="H8" s="116"/>
+      <c r="H8" s="115"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="110" t="s">
+      <c r="A9" t="s">
         <v>308</v>
       </c>
       <c r="B9">
@@ -33693,7 +33686,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="110" t="s">
+      <c r="A10" t="s">
         <v>309</v>
       </c>
       <c r="B10">
@@ -33716,7 +33709,7 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11">
@@ -33739,13 +33732,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>310</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12">
         <v>2.7</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12">
         <v>0.85</v>
       </c>
       <c r="D12">
@@ -33762,14 +33755,14 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>311</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13">
         <f>B12</f>
         <v>2.7</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13">
         <v>0.61</v>
       </c>
       <c r="D13">
@@ -33786,13 +33779,13 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>312</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14">
         <v>1.5</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14">
         <v>0.4</v>
       </c>
       <c r="D14">
@@ -33809,13 +33802,13 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
         <v>0.74</v>
       </c>
       <c r="D15">
@@ -33832,13 +33825,13 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16">
         <v>4.5</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16">
         <v>0.43</v>
       </c>
       <c r="D16">

</xml_diff>